<commit_message>
LiteralValues ContextRestriction + fixes in parsing and token-suggesting for some corner cases
</commit_message>
<xml_diff>
--- a/tratto/src/test/resources/oracles-dataset.xlsx
+++ b/tratto/src/test/resources/oracles-dataset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alberto/workspace/STAR/StarLab/Projects/ASTERIX/Oracle/Implementation/dataset-tokens/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alberto/workspace/STAR/tratto/tratto/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B583D4-91C1-6341-913E-5F9F106C3A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F3E66C-1DAB-2147-9811-95E2B045A88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{02EBD5D7-2F3A-A74C-B78E-C1F986350E2F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72">
   <si>
     <t>projectName</t>
   </si>
@@ -1561,7 +1561,10 @@
     <t>[RealFieldElement;org.apache.commons.math3],[Primes;org.apache.commons.math3.primes],[DifferentiableUnivariateFunction;org.apache.commons.math3.analysis],[UnivariateFunction;org.apache.commons.math3.analysis],[TrivariateFunction;org.apache.commons.math3.analysis],[MultivariateMatrixFunction;org.apache.commons.math3.analysis],[ParametricUnivariateFunction;org.apache.commons.math3.analysis],[UnivariateDifferentiableVectorFunction;org.apache.commons.math3.analysis.differentiation],[UnivariateDifferentiableMatrixFunction;org.apache.commons.math3.analysis.differentiation],[DSCompiler;org.apache.commons.math3.analysis.differentiation],[SparseGradient;org.apache.commons.math3.analysis.differentiation],[UnivariateFunctionDifferentiator;org.apache.commons.math3.analysis.differentiation],[UnivariateDifferentiableFunction;org.apache.commons.math3.analysis.differentiation],[MultivariateVectorFunction;org.apache.commons.math3.analysis],[DifferentiableMultivariateVectorFunction;org.apache.commons.math3.analysis],[PolynomialFunctionNewtonForm;org.apache.commons.math3.analysis.polynomials],[PolynomialFunctionLagrangeForm;org.apache.commons.math3.analysis.polynomials],[PolynomialSplineFunction;org.apache.commons.math3.analysis.polynomials],[PolynomialsUtils;org.apache.commons.math3.analysis.polynomials],[PolynomialFunction;org.apache.commons.math3.analysis.polynomials],[Complex;org.apache.commons.math3.complex],[Field; org.apache.commons.math3],[FieldElement;org.apache.commons.math3],[DerivativeStructure;org.apache.commons.math3.analysis.differentiation]</t>
   </si>
   <si>
-    <t>[List; java.util], [AbstractBagDecorator; package.name.here], [CollectionBag; org.apache.commons.collections4.bag], [CollectionSortedBag; package.name.here], [DefaultEquator; package.name.here], [AbstractPropertiesFactory; package.name.here], [PropertiesFactory; package.name.here], [SortedProperties; package.name.here], [SortedPropertiesFactory; package.name.here], [ArrayUtils; package.name.here], [Bag; org.apache.commons.collections4], [BagUtils; org.apache.commons.collections4], [BidiMap; package.name.here], [BoundedCollection; package.name.here], [BoundedMap; package.name.here], [Closure; package.name.here], [ClosureUtils; package.name.here], [CollectionUtils; package.name.here], [ComparatorUtils; package.name.here], [EnumerationUtils; package.name.here], [Equator; package.name.here]</t>
+    <t>[Boolean; java.lang], [String; java.lang], [List; java.util], [AbstractBagDecorator; package.name.here], [CollectionBag; org.apache.commons.collections4.bag], [CollectionSortedBag; package.name.here], [DefaultEquator; package.name.here], [AbstractPropertiesFactory; package.name.here], [PropertiesFactory; package.name.here], [SortedProperties; package.name.here], [SortedPropertiesFactory; package.name.here], [ArrayUtils; package.name.here], [Bag; org.apache.commons.collections4], [BagUtils; org.apache.commons.collections4], [BidiMap; package.name.here], [BoundedCollection; package.name.here], [BoundedMap; package.name.here], [Closure; package.name.here], [ClosureUtils; package.name.here], [CollectionUtils; package.name.here], [ComparatorUtils; package.name.here], [EnumerationUtils; package.name.here], [Equator; package.name.here]</t>
+  </si>
+  <si>
+    <t>[3.1; double]</t>
   </si>
 </sst>
 </file>
@@ -1920,8 +1923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A0D715B-BCC9-BF43-809F-F5D4ACB402A1}">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="125" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="P2" zoomScale="125" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2075,7 +2078,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2124,6 +2127,9 @@
       </c>
       <c r="P3" t="s">
         <v>25</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>71</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
Handle automatically expressions using jdVar (e.g., when getting return type)
Close #10
</commit_message>
<xml_diff>
--- a/tratto/src/test/resources/oracles-dataset.xlsx
+++ b/tratto/src/test/resources/oracles-dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alberto/workspace/STAR/tratto/tratto/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F3E66C-1DAB-2147-9811-95E2B045A88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE82801-C775-7A42-B3CB-8FA93AA7C4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{02EBD5D7-2F3A-A74C-B78E-C1F986350E2F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
   <si>
     <t>projectName</t>
   </si>
@@ -1565,6 +1565,70 @@
   </si>
   <si>
     <t>[3.1; double]</t>
+  </si>
+  <si>
+    <t>true ? methodResultID.stream().noneMatch(jdVar -&gt; jdVar == null) : true;</t>
+  </si>
+  <si>
+    <t>@return a List of all {@code n}-th roots of {@code this}.</t>
+  </si>
+  <si>
+    <t>/**
+     * Computes the n-th roots of this complex number.
+     * The nth roots are defined by the formula:
+     * &lt;pre&gt;
+     *  &lt;code&gt;
+     *   z&lt;sub&gt;k&lt;/sub&gt; = abs&lt;sup&gt;1/n&lt;/sup&gt; (cos(phi + 2&amp;pi;k/n) + i (sin(phi + 2&amp;pi;k/n))
+     *  &lt;/code&gt;
+     * &lt;/pre&gt;
+     * for &lt;i&gt;{@code k=0, 1, ..., n-1}&lt;/i&gt;, where {@code abs} and {@code phi}
+     * are respectively the {@link #abs() modulus} and
+     * {@link #getArgument() argument} of this complex number.
+     * &lt;p&gt;
+     * If one or both parts of this complex number is NaN, a list with just
+     * one element, {@link #NaN} is returned.
+     * if neither part is NaN, but at least one part is infinite, the result
+     * is a one-element list containing {@link #INF}.
+     *
+     * @param n Degree of root.
+     * @return a List of all {@code n}-th roots of {@code this}.
+     * @throws NotPositiveException if {@code n &lt;= 0}.
+     * @since 2.0
+     */</t>
+  </si>
+  <si>
+    <t>public List&lt;Complex&gt; nthRoot(int n) throws NotPositiveException {
+        if (n &lt;= 0) {
+            throw new NotPositiveException(LocalizedFormats.CANNOT_COMPUTE_NTH_ROOT_FOR_NEGATIVE_N,
+                                           n);
+        }
+        final List&lt;Complex&gt; result = new ArrayList&lt;Complex&gt;();
+        if (isNaN) {
+            result.add(NaN);
+            return result;
+        }
+        if (isInfinite()) {
+            result.add(INF);
+            return result;
+        }
+        // nth root of abs -- faster / more accurate to use a solver here?
+        final double nthRootOfAbs = FastMath.pow(abs(), 1.0 / n);
+        // Compute nth roots of complex number with k = 0, 1, ... n-1
+        final double nthPhi = getArgument() / n;
+        final double slice = 2 * FastMath.PI / n;
+        double innerPart = nthPhi;
+        for (int k = 0; k &lt; n ; k++) {
+            // inner part
+            final double realPart = nthRootOfAbs *  FastMath.cos(innerPart);
+            final double imaginaryPart = nthRootOfAbs *  FastMath.sin(innerPart);
+            result.add(createComplex(realPart, imaginaryPart));
+            innerPart += slice;
+        }
+        return result;
+    }</t>
+  </si>
+  <si>
+    <t>[n; ; int]</t>
   </si>
 </sst>
 </file>
@@ -1921,10 +1985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A0D715B-BCC9-BF43-809F-F5D4ACB402A1}">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P2" zoomScale="125" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" topLeftCell="S5" zoomScale="125" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2262,6 +2326,65 @@
         <v>62</v>
       </c>
     </row>
+    <row r="6" spans="1:22" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P6" t="s">
+        <v>63</v>
+      </c>
+      <c r="R6" t="s">
+        <v>76</v>
+      </c>
+      <c r="S6" t="s">
+        <v>68</v>
+      </c>
+      <c r="T6" t="s">
+        <v>66</v>
+      </c>
+      <c r="U6" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Handle arguments of Arrays.stream() via TokenEnricher and new ContextRestriction
</commit_message>
<xml_diff>
--- a/tratto/src/test/resources/oracles-dataset.xlsx
+++ b/tratto/src/test/resources/oracles-dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alberto/workspace/STAR/tratto/tratto/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67548C89-BFE6-4048-8BDD-27767A579025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FAC81F-A5B7-9140-B87D-2E934A7BCD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{02EBD5D7-2F3A-A74C-B78E-C1F986350E2F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{02EBD5D7-2F3A-A74C-B78E-C1F986350E2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="84">
   <si>
     <t>projectName</t>
   </si>
@@ -1632,6 +1632,46 @@
   </si>
   <si>
     <t>[isInfinite; org.apache.commons.math3.complex; Complex; public boolean isInfinite()], [isNaN; org.apache.commons.math3.complex; Complex; public boolean isNaN()], [stream; java.util; Collection; public Stream&lt;E&gt;  stream()], [equals; java.lang; Object; public boolean equals(Object obj)], [toString; java.lang; Object; public String toString()], [getClass; java.lang; Object; public final native Class&lt;?&gt; getClass()], [hashCode; java.lang; Object; public native int hashCode()], [hash; org.apache.commons.collections4; Equator; int hash(T o)]</t>
+  </si>
+  <si>
+    <t>true ? Arrays.stream(coefficients).noneMatch(jdVar -&gt; jdVar == null) : true;</t>
+  </si>
+  <si>
+    <t>@return the coefficients of the derivative or {@code null} if coefficients has length 1.</t>
+  </si>
+  <si>
+    <t>/**
+     * Returns the coefficients of the derivative of the polynomial with the given coefficients.
+     *
+     * @param coefficients Coefficients of the polynomial to differentiate.
+     * @return the coefficients of the derivative or {@code null} if coefficients has length 1.
+     * @throws NoDataException if {@code coefficients} is empty.
+     * @throws NullArgumentException if {@code coefficients} is {@code null}.
+     */</t>
+  </si>
+  <si>
+    <t>protected static double[] differentiate(double[] coefficients)
+        throws NullArgumentException, NoDataException {
+        MathUtils.checkNotNull(coefficients);
+        int n = coefficients.length;
+        if (n == 0) {
+            throw new NoDataException(LocalizedFormats.EMPTY_POLYNOMIALS_COEFFICIENTS_ARRAY);
+        }
+        if (n == 1) {
+            return new double[]{0};
+        }
+        double[] result = new double[n - 1];
+        for (int i = n - 1; i &gt; 0; i--) {
+            result[i - 1] = i * coefficients[i];
+        }
+        return result;
+    }</t>
+  </si>
+  <si>
+    <t>[1; int]</t>
+  </si>
+  <si>
+    <t>[coefficients;;double\[\]]</t>
   </si>
 </sst>
 </file>
@@ -1988,10 +2028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A0D715B-BCC9-BF43-809F-F5D4ACB402A1}">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q6" zoomScale="125" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" topLeftCell="S6" zoomScale="125" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2388,6 +2428,67 @@
         <v>62</v>
       </c>
     </row>
+    <row r="7" spans="1:22" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>82</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
NoClass ContextRestriction + tests for some more corner cases
</commit_message>
<xml_diff>
--- a/tratto/src/test/resources/oracles-dataset.xlsx
+++ b/tratto/src/test/resources/oracles-dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alberto/workspace/STAR/tratto/tratto/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FAC81F-A5B7-9140-B87D-2E934A7BCD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A3AEEE-D60A-A745-A371-94FDA39FEB98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{02EBD5D7-2F3A-A74C-B78E-C1F986350E2F}"/>
   </bookViews>
@@ -2030,8 +2030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A0D715B-BCC9-BF43-809F-F5D4ACB402A1}">
   <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S6" zoomScale="125" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+    <sheetView tabSelected="1" topLeftCell="G4" zoomScale="125" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>